<commit_message>
modified bulletcreate,enemy status.add script damege_font,damege Calculation
</commit_message>
<xml_diff>
--- a/ItemData..xlsx
+++ b/ItemData..xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="ItemData" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ItemData!$A$1:$S$18</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -27,112 +30,112 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Endurance</t>
+  </si>
+  <si>
+    <t>Dexterity</t>
+  </si>
+  <si>
+    <t>Perception</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>Magical_power</t>
+  </si>
+  <si>
+    <t>Charisma</t>
+  </si>
+  <si>
+    <t>Agility</t>
+  </si>
+  <si>
+    <t>Luck</t>
+  </si>
+  <si>
+    <t>Stamina</t>
+  </si>
+  <si>
+    <t>Satiety</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>"Nothing"</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>"It's red vegiable"</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>Carrot</t>
+  </si>
+  <si>
+    <t>Artichoke</t>
+  </si>
+  <si>
+    <t>Chilli</t>
+  </si>
+  <si>
+    <t>Gourd</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>Bucket</t>
+  </si>
+  <si>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t>Picture</t>
+  </si>
+  <si>
+    <t>Axe</t>
+  </si>
+  <si>
+    <t>Potion</t>
+  </si>
+  <si>
+    <t>Starfish</t>
+  </si>
+  <si>
+    <t>Mushroom</t>
+  </si>
+  <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>HP</t>
-  </si>
-  <si>
-    <t>MP</t>
-  </si>
-  <si>
-    <t>Strength</t>
-  </si>
-  <si>
-    <t>Endurance</t>
-  </si>
-  <si>
-    <t>Dexterity</t>
-  </si>
-  <si>
-    <t>Perception</t>
-  </si>
-  <si>
-    <t>Master</t>
-  </si>
-  <si>
-    <t>Will</t>
-  </si>
-  <si>
-    <t>Magical_power</t>
-  </si>
-  <si>
-    <t>Charisma</t>
-  </si>
-  <si>
-    <t>Agility</t>
-  </si>
-  <si>
-    <t>Luck</t>
-  </si>
-  <si>
-    <t>Stamina</t>
-  </si>
-  <si>
-    <t>Satiety</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Nothing</t>
-  </si>
-  <si>
-    <t>"Nothing"</t>
-  </si>
-  <si>
-    <t>Tomato</t>
-  </si>
-  <si>
-    <t>"It's red vegiable"</t>
-  </si>
-  <si>
-    <t>Potato</t>
-  </si>
-  <si>
-    <t>Carrot</t>
-  </si>
-  <si>
-    <t>Artichoke</t>
-  </si>
-  <si>
-    <t>Chilli</t>
-  </si>
-  <si>
-    <t>Gourd</t>
-  </si>
-  <si>
-    <t>Corn</t>
-  </si>
-  <si>
-    <t>Wood</t>
-  </si>
-  <si>
-    <t>Stone</t>
-  </si>
-  <si>
-    <t>Bucket</t>
-  </si>
-  <si>
-    <t>Chair</t>
-  </si>
-  <si>
-    <t>Picture</t>
-  </si>
-  <si>
-    <t>Axe</t>
-  </si>
-  <si>
-    <t>Potion</t>
-  </si>
-  <si>
-    <t>Starfish</t>
-  </si>
-  <si>
-    <t>Mushroom</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1056,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1066,55 +1069,55 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
@@ -1122,58 +1125,58 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
         <v>19</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.15">
@@ -1181,7 +1184,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1232,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
@@ -1240,7 +1243,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1296,7 +1299,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1352,7 +1355,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1408,7 +1411,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1464,7 +1467,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1520,7 +1523,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1576,7 +1579,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -1632,7 +1635,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -1688,7 +1691,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1744,7 +1747,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -1800,7 +1803,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -1856,7 +1859,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -1912,7 +1915,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1968,7 +1971,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2024,7 +2027,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2078,5 +2081,6 @@
   </sheetData>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add player status.Equipment.well fix damege_create system
</commit_message>
<xml_diff>
--- a/ItemData..xlsx
+++ b/ItemData..xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naoto10\Documents\GameMakerStudio2\shooting3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\naoto\GameMaker2\shooting3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="ItemData" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ItemData!$A$1:$S$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ItemData!$A$1:$U$18</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>ItemID</t>
   </si>
@@ -136,12 +136,20 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>MaxHP</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>MaxMP</t>
+    <phoneticPr fontId="18"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1053,15 +1061,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1075,52 +1083,58 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1175,11 +1189,17 @@
       <c r="R2">
         <v>0</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1193,11 +1213,11 @@
         <v>0.1</v>
       </c>
       <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
       <c r="G3">
         <v>0</v>
       </c>
@@ -1234,11 +1254,17 @@
       <c r="R3">
         <v>0</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1252,11 +1278,11 @@
         <v>0.1</v>
       </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>9</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
       <c r="G4">
         <v>0</v>
       </c>
@@ -1293,8 +1319,14 @@
       <c r="R4">
         <v>0</v>
       </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1308,11 +1340,11 @@
         <v>0.1</v>
       </c>
       <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>8</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
       <c r="G5">
         <v>0</v>
       </c>
@@ -1349,8 +1381,14 @@
       <c r="R5">
         <v>0</v>
       </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1364,11 +1402,11 @@
         <v>0.1</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>7</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
       <c r="G6">
         <v>0</v>
       </c>
@@ -1405,8 +1443,14 @@
       <c r="R6">
         <v>0</v>
       </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1420,11 +1464,11 @@
         <v>0.1</v>
       </c>
       <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>6</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
       <c r="G7">
         <v>0</v>
       </c>
@@ -1461,8 +1505,14 @@
       <c r="R7">
         <v>0</v>
       </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1476,11 +1526,11 @@
         <v>0.1</v>
       </c>
       <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>5</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
       <c r="G8">
         <v>0</v>
       </c>
@@ -1517,8 +1567,14 @@
       <c r="R8">
         <v>0</v>
       </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1532,11 +1588,11 @@
         <v>0.1</v>
       </c>
       <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>4</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
       <c r="G9">
         <v>0</v>
       </c>
@@ -1573,8 +1629,14 @@
       <c r="R9">
         <v>0</v>
       </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1582,7 +1644,7 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1629,8 +1691,14 @@
       <c r="R10">
         <v>0</v>
       </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1638,7 +1706,7 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1685,8 +1753,14 @@
       <c r="R11">
         <v>0</v>
       </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1694,7 +1768,7 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -1741,8 +1815,14 @@
       <c r="R12">
         <v>0</v>
       </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1750,7 +1830,7 @@
         <v>31</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -1797,8 +1877,14 @@
       <c r="R13">
         <v>0</v>
       </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1806,7 +1892,7 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>0.1</v>
@@ -1853,8 +1939,14 @@
       <c r="R14">
         <v>0</v>
       </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1862,7 +1954,7 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -1909,8 +2001,14 @@
       <c r="R15">
         <v>0</v>
       </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1924,11 +2022,11 @@
         <v>0.1</v>
       </c>
       <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
         <v>100</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
       <c r="G16">
         <v>0</v>
       </c>
@@ -1965,8 +2063,14 @@
       <c r="R16">
         <v>0</v>
       </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1980,11 +2084,11 @@
         <v>0.1</v>
       </c>
       <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
         <v>5</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
       <c r="G17">
         <v>0</v>
       </c>
@@ -2021,8 +2125,14 @@
       <c r="R17">
         <v>0</v>
       </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2036,11 +2146,11 @@
         <v>0.5</v>
       </c>
       <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
         <v>30</v>
       </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
       <c r="G18">
         <v>0</v>
       </c>
@@ -2075,6 +2185,12 @@
         <v>0</v>
       </c>
       <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix scr_use_item.add prottype equip_item_script.
</commit_message>
<xml_diff>
--- a/ItemData..xlsx
+++ b/ItemData..xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\naoto\GameMaker2\shooting3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naoto10\Documents\GameMakerStudio2\shooting3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ItemData!$A$1:$U$18</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>ItemID</t>
   </si>
@@ -139,17 +139,21 @@
   </si>
   <si>
     <t>MaxHP</t>
-    <phoneticPr fontId="18"/>
   </si>
   <si>
     <t>MaxMP</t>
-    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>MaxSatiety</t>
+  </si>
+  <si>
+    <t>"test advantege"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1061,7 +1065,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -1069,7 +1073,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1095,46 +1099,49 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1195,11 +1202,14 @@
       <c r="T2">
         <v>0</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1252,19 +1262,22 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
         <v>0</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1325,8 +1338,11 @@
       <c r="T4">
         <v>0</v>
       </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1387,8 +1403,11 @@
       <c r="T5">
         <v>0</v>
       </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1449,8 +1468,11 @@
       <c r="T6">
         <v>0</v>
       </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1511,8 +1533,11 @@
       <c r="T7">
         <v>0</v>
       </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1573,8 +1598,11 @@
       <c r="T8">
         <v>0</v>
       </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1588,7 +1616,7 @@
         <v>0.1</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -1635,8 +1663,14 @@
       <c r="T9">
         <v>0</v>
       </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1697,8 +1731,11 @@
       <c r="T10">
         <v>0</v>
       </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1759,8 +1796,11 @@
       <c r="T11">
         <v>0</v>
       </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1821,8 +1861,11 @@
       <c r="T12">
         <v>0</v>
       </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1883,8 +1926,11 @@
       <c r="T13">
         <v>0</v>
       </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1898,7 +1944,7 @@
         <v>0.1</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1945,8 +1991,11 @@
       <c r="T14">
         <v>0</v>
       </c>
+      <c r="U14">
+        <v>50</v>
+      </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1960,7 +2009,7 @@
         <v>5</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -2007,8 +2056,11 @@
       <c r="T15">
         <v>0</v>
       </c>
+      <c r="U15">
+        <v>100</v>
+      </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2069,8 +2121,11 @@
       <c r="T16">
         <v>0</v>
       </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2131,8 +2186,11 @@
       <c r="T17">
         <v>0</v>
       </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2191,6 +2249,9 @@
         <v>0</v>
       </c>
       <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
         <v>0</v>
       </c>
     </row>

</xml_diff>